<commit_message>
se agregan los datos de semana, entre 7 y 11 de febrero
</commit_message>
<xml_diff>
--- a/datos/cambios_de_estado_de_cita.xlsx
+++ b/datos/cambios_de_estado_de_cita.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositorios\estadistica_agendamientos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositorios\estadistica_agendamientos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D9D17A-0370-43E2-BCA8-80D19811B079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7518E7-C27B-49C4-AF04-BEEF80E75666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Recepcionista</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>07_02_2024</t>
+  </si>
+  <si>
+    <t>11_02_2024</t>
   </si>
 </sst>
 </file>
@@ -375,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -388,7 +391,7 @@
     <col min="3" max="3" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,8 +413,11 @@
       <c r="G1" t="s">
         <v>10</v>
       </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -433,8 +439,11 @@
       <c r="G2">
         <v>3063</v>
       </c>
+      <c r="H2">
+        <v>3215</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -456,8 +465,11 @@
       <c r="G3">
         <v>2314</v>
       </c>
+      <c r="H3">
+        <v>2385</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -479,8 +491,11 @@
       <c r="G4">
         <v>3618</v>
       </c>
+      <c r="H4">
+        <v>3682</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -501,6 +516,9 @@
       </c>
       <c r="G5">
         <v>6927</v>
+      </c>
+      <c r="H5">
+        <v>6931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregada una nueva recepcionista y los datos de semana 18/02/2024
</commit_message>
<xml_diff>
--- a/datos/cambios_de_estado_de_cita.xlsx
+++ b/datos/cambios_de_estado_de_cita.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositorios\estadistica_agendamientos\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\estadistica_agendamientos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7518E7-C27B-49C4-AF04-BEEF80E75666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E03246-48A8-4A8E-A6F9-DE093464ECDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Recepcionista</t>
   </si>
@@ -61,14 +61,28 @@
   </si>
   <si>
     <t>11_02_2024</t>
+  </si>
+  <si>
+    <t>Constanza</t>
+  </si>
+  <si>
+    <t>18_02_2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -96,8 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -391,7 +406,7 @@
     <col min="3" max="3" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,8 +431,11 @@
       <c r="H1" t="s">
         <v>11</v>
       </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -442,8 +460,11 @@
       <c r="H2">
         <v>3215</v>
       </c>
+      <c r="I2">
+        <v>3215</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -468,8 +489,11 @@
       <c r="H3">
         <v>2385</v>
       </c>
+      <c r="I3" s="1">
+        <v>2640</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -494,8 +518,11 @@
       <c r="H4">
         <v>3682</v>
       </c>
+      <c r="I4">
+        <v>3769</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -519,9 +546,42 @@
       </c>
       <c r="H5">
         <v>6931</v>
+      </c>
+      <c r="I5">
+        <v>7034</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mejor organización de datos
</commit_message>
<xml_diff>
--- a/datos/cambios_de_estado_de_cita.xlsx
+++ b/datos/cambios_de_estado_de_cita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\estadistica_agendamientos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E03246-48A8-4A8E-A6F9-DE093464ECDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C0860C-5E4D-4347-A0AA-9C880317DC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Recepcionista</t>
   </si>
@@ -40,24 +40,6 @@
   </si>
   <si>
     <t>Felipe</t>
-  </si>
-  <si>
-    <t>18_12_2023</t>
-  </si>
-  <si>
-    <t>05_01_2024</t>
-  </si>
-  <si>
-    <t>15_01_2024</t>
-  </si>
-  <si>
-    <t>21_01_2024</t>
-  </si>
-  <si>
-    <t>28_01_2024</t>
-  </si>
-  <si>
-    <t>07_02_2024</t>
   </si>
   <si>
     <t>11_02_2024</t>
@@ -393,20 +375,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,169 +394,61 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1826</v>
+        <v>3215</v>
       </c>
       <c r="C2">
-        <v>2293</v>
-      </c>
-      <c r="D2">
-        <v>2525</v>
-      </c>
-      <c r="E2">
-        <v>2638</v>
-      </c>
-      <c r="F2">
-        <v>2824</v>
-      </c>
-      <c r="G2">
-        <v>3063</v>
-      </c>
-      <c r="H2">
         <v>3215</v>
       </c>
-      <c r="I2">
-        <v>3215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1269</v>
-      </c>
-      <c r="C3">
-        <v>1716</v>
-      </c>
-      <c r="D3">
-        <v>1910</v>
-      </c>
-      <c r="E3">
-        <v>2032</v>
-      </c>
-      <c r="F3">
-        <v>2097</v>
-      </c>
-      <c r="G3">
-        <v>2314</v>
-      </c>
-      <c r="H3">
         <v>2385</v>
       </c>
-      <c r="I3" s="1">
+      <c r="C3" s="1">
         <v>2640</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3019</v>
+        <v>3682</v>
       </c>
       <c r="C4">
-        <v>3196</v>
-      </c>
-      <c r="D4">
-        <v>3373</v>
-      </c>
-      <c r="E4">
-        <v>3446</v>
-      </c>
-      <c r="F4">
-        <v>3537</v>
-      </c>
-      <c r="G4">
-        <v>3618</v>
-      </c>
-      <c r="H4">
-        <v>3682</v>
-      </c>
-      <c r="I4">
         <v>3769</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>6672</v>
+        <v>6931</v>
       </c>
       <c r="C5">
-        <v>6688</v>
-      </c>
-      <c r="D5">
-        <v>6704</v>
-      </c>
-      <c r="E5">
-        <v>6784</v>
-      </c>
-      <c r="F5">
-        <v>6858</v>
-      </c>
-      <c r="G5">
-        <v>6927</v>
-      </c>
-      <c r="H5">
-        <v>6931</v>
-      </c>
-      <c r="I5">
         <v>7034</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
puesto en una rama antigua
</commit_message>
<xml_diff>
--- a/datos/cambios_de_estado_de_cita.xlsx
+++ b/datos/cambios_de_estado_de_cita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\estadistica_agendamientos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C0860C-5E4D-4347-A0AA-9C880317DC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E03246-48A8-4A8E-A6F9-DE093464ECDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Recepcionista</t>
   </si>
@@ -40,6 +40,24 @@
   </si>
   <si>
     <t>Felipe</t>
+  </si>
+  <si>
+    <t>18_12_2023</t>
+  </si>
+  <si>
+    <t>05_01_2024</t>
+  </si>
+  <si>
+    <t>15_01_2024</t>
+  </si>
+  <si>
+    <t>21_01_2024</t>
+  </si>
+  <si>
+    <t>28_01_2024</t>
+  </si>
+  <si>
+    <t>07_02_2024</t>
   </si>
   <si>
     <t>11_02_2024</t>
@@ -375,18 +393,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,61 +414,169 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>1826</v>
+      </c>
+      <c r="C2">
+        <v>2293</v>
+      </c>
+      <c r="D2">
+        <v>2525</v>
+      </c>
+      <c r="E2">
+        <v>2638</v>
+      </c>
+      <c r="F2">
+        <v>2824</v>
+      </c>
+      <c r="G2">
+        <v>3063</v>
+      </c>
+      <c r="H2">
         <v>3215</v>
       </c>
-      <c r="C2">
+      <c r="I2">
         <v>3215</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>1269</v>
+      </c>
+      <c r="C3">
+        <v>1716</v>
+      </c>
+      <c r="D3">
+        <v>1910</v>
+      </c>
+      <c r="E3">
+        <v>2032</v>
+      </c>
+      <c r="F3">
+        <v>2097</v>
+      </c>
+      <c r="G3">
+        <v>2314</v>
+      </c>
+      <c r="H3">
         <v>2385</v>
       </c>
-      <c r="C3" s="1">
+      <c r="I3" s="1">
         <v>2640</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>3019</v>
+      </c>
+      <c r="C4">
+        <v>3196</v>
+      </c>
+      <c r="D4">
+        <v>3373</v>
+      </c>
+      <c r="E4">
+        <v>3446</v>
+      </c>
+      <c r="F4">
+        <v>3537</v>
+      </c>
+      <c r="G4">
+        <v>3618</v>
+      </c>
+      <c r="H4">
         <v>3682</v>
       </c>
-      <c r="C4">
+      <c r="I4">
         <v>3769</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>6672</v>
+      </c>
+      <c r="C5">
+        <v>6688</v>
+      </c>
+      <c r="D5">
+        <v>6704</v>
+      </c>
+      <c r="E5">
+        <v>6784</v>
+      </c>
+      <c r="F5">
+        <v>6858</v>
+      </c>
+      <c r="G5">
+        <v>6927</v>
+      </c>
+      <c r="H5">
         <v>6931</v>
       </c>
-      <c r="C5">
+      <c r="I5">
         <v>7034</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrega los datos de agendamiento de semana del 19 de feb, además de las pruebas de agendamiento
</commit_message>
<xml_diff>
--- a/datos/cambios_de_estado_de_cita.xlsx
+++ b/datos/cambios_de_estado_de_cita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\estadistica_agendamientos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C0860C-5E4D-4347-A0AA-9C880317DC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD081AB0-5299-44AC-AF94-57C51BC1029E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Recepcionista</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>18_02_2024</t>
+  </si>
+  <si>
+    <t>25_02_2024</t>
   </si>
 </sst>
 </file>
@@ -375,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -386,7 +389,7 @@
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -396,8 +399,11 @@
       <c r="C1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -407,8 +413,11 @@
       <c r="C2">
         <v>3215</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>3414</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -418,8 +427,11 @@
       <c r="C3" s="1">
         <v>2640</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>2769</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -429,8 +441,11 @@
       <c r="C4">
         <v>3769</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>3919</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -440,8 +455,11 @@
       <c r="C5">
         <v>7034</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>7058</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -450,6 +468,9 @@
       </c>
       <c r="C6">
         <v>33</v>
+      </c>
+      <c r="D6">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambio de estado de cita 26 feb
</commit_message>
<xml_diff>
--- a/datos/cambios_de_estado_de_cita.xlsx
+++ b/datos/cambios_de_estado_de_cita.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\estadistica_agendamientos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD081AB0-5299-44AC-AF94-57C51BC1029E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E700F46-D9CC-48E7-96D9-A320801625CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,18 +379,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,8 +404,11 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
+      <c r="E1" s="2">
+        <v>45354</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -416,8 +421,11 @@
       <c r="D2">
         <v>3414</v>
       </c>
+      <c r="E2">
+        <v>3545</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -430,8 +438,11 @@
       <c r="D3">
         <v>2769</v>
       </c>
+      <c r="E3">
+        <v>2975</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -444,8 +455,11 @@
       <c r="D4">
         <v>3919</v>
       </c>
+      <c r="E4">
+        <v>4050</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -458,8 +472,11 @@
       <c r="D5">
         <v>7058</v>
       </c>
+      <c r="E5">
+        <v>7118</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -471,6 +488,9 @@
       </c>
       <c r="D6">
         <v>137</v>
+      </c>
+      <c r="E6">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no sé si está funcionando
</commit_message>
<xml_diff>
--- a/datos/cambios_de_estado_de_cita.xlsx
+++ b/datos/cambios_de_estado_de_cita.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\estadistica_agendamientos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E700F46-D9CC-48E7-96D9-A320801625CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9356BA5B-8AC1-4F81-9517-E495A8AC6CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Recepcionista</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>25_02_2024</t>
+  </si>
+  <si>
+    <t>03_03_2024</t>
   </si>
 </sst>
 </file>
@@ -382,7 +385,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,8 +407,8 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2">
-        <v>45354</v>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
se agregan los datos de agendamiento en los excel
</commit_message>
<xml_diff>
--- a/datos/cambios_de_estado_de_cita.xlsx
+++ b/datos/cambios_de_estado_de_cita.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\estadistica_agendamientos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9356BA5B-8AC1-4F81-9517-E495A8AC6CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0186D3A7-0CB4-47EE-A7CB-8A801802FABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Recepcionista</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>03_03_2024</t>
+  </si>
+  <si>
+    <t>11_03_2024</t>
   </si>
 </sst>
 </file>
@@ -382,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -394,7 +397,7 @@
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,8 +413,11 @@
       <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -427,8 +433,11 @@
       <c r="E2">
         <v>3545</v>
       </c>
+      <c r="F2">
+        <v>3732</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -444,8 +453,11 @@
       <c r="E3">
         <v>2975</v>
       </c>
+      <c r="F3">
+        <v>3189</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -461,8 +473,11 @@
       <c r="E4">
         <v>4050</v>
       </c>
+      <c r="F4">
+        <v>4192</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -478,8 +493,11 @@
       <c r="E5">
         <v>7118</v>
       </c>
+      <c r="F5">
+        <v>7163</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -494,6 +512,9 @@
       </c>
       <c r="E6">
         <v>216</v>
+      </c>
+      <c r="F6">
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agregan los datos de semana del 11 de marzo
</commit_message>
<xml_diff>
--- a/datos/cambios_de_estado_de_cita.xlsx
+++ b/datos/cambios_de_estado_de_cita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\estadistica_agendamientos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0186D3A7-0CB4-47EE-A7CB-8A801802FABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D981DFC-C771-469E-A1BC-AD0586F7A1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Recepcionista</t>
   </si>
@@ -39,18 +39,9 @@
     <t>Betty</t>
   </si>
   <si>
-    <t>Felipe</t>
-  </si>
-  <si>
-    <t>11_02_2024</t>
-  </si>
-  <si>
     <t>Constanza</t>
   </si>
   <si>
-    <t>18_02_2024</t>
-  </si>
-  <si>
     <t>25_02_2024</t>
   </si>
   <si>
@@ -58,22 +49,17 @@
   </si>
   <si>
     <t>11_03_2024</t>
+  </si>
+  <si>
+    <t>17_03_2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,9 +87,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -385,136 +370,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3215</v>
+        <v>3414</v>
       </c>
       <c r="C2">
-        <v>3215</v>
+        <v>3545</v>
       </c>
       <c r="D2">
-        <v>3414</v>
+        <v>3732</v>
       </c>
       <c r="E2">
-        <v>3545</v>
-      </c>
-      <c r="F2">
-        <v>3732</v>
+        <v>3979</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2385</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2640</v>
+        <v>2769</v>
+      </c>
+      <c r="C3">
+        <v>2975</v>
       </c>
       <c r="D3">
-        <v>2769</v>
+        <v>3189</v>
       </c>
       <c r="E3">
-        <v>2975</v>
-      </c>
-      <c r="F3">
-        <v>3189</v>
+        <v>3327</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3682</v>
+        <v>3919</v>
       </c>
       <c r="C4">
-        <v>3769</v>
+        <v>4050</v>
       </c>
       <c r="D4">
-        <v>3919</v>
+        <v>4192</v>
       </c>
       <c r="E4">
-        <v>4050</v>
-      </c>
-      <c r="F4">
-        <v>4192</v>
+        <v>4273</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>6931</v>
+        <v>137</v>
       </c>
       <c r="C5">
-        <v>7034</v>
+        <v>216</v>
       </c>
       <c r="D5">
-        <v>7058</v>
+        <v>363</v>
       </c>
       <c r="E5">
-        <v>7118</v>
-      </c>
-      <c r="F5">
-        <v>7163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>33</v>
-      </c>
-      <c r="D6">
-        <v>137</v>
-      </c>
-      <c r="E6">
-        <v>216</v>
-      </c>
-      <c r="F6">
-        <v>363</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualización de datos hasta 25 de marzo
</commit_message>
<xml_diff>
--- a/datos/cambios_de_estado_de_cita.xlsx
+++ b/datos/cambios_de_estado_de_cita.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\estadistica_agendamientos\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D981DFC-C771-469E-A1BC-AD0586F7A1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57761CBD-8C13-4901-93C0-A88F0067A02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Recepcionista</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>17_03_2024</t>
+  </si>
+  <si>
+    <t>26_03_2024</t>
   </si>
 </sst>
 </file>
@@ -370,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,7 +385,7 @@
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,8 +401,11 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -415,8 +421,11 @@
       <c r="E2">
         <v>3979</v>
       </c>
+      <c r="F2">
+        <v>4247</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -432,8 +441,11 @@
       <c r="E3">
         <v>3327</v>
       </c>
+      <c r="F3">
+        <v>3546</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -449,8 +461,11 @@
       <c r="E4">
         <v>4273</v>
       </c>
+      <c r="F4">
+        <v>4411</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -465,6 +480,9 @@
       </c>
       <c r="E5">
         <v>440</v>
+      </c>
+      <c r="F5">
+        <v>548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>